<commit_message>
Moved some todo stuff to spreadsheet
</commit_message>
<xml_diff>
--- a/progress/spreadsheet/spreadsheet.xlsx
+++ b/progress/spreadsheet/spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\progress\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B67FFA-2361-4176-90BD-053C88E3CE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ACF646-C629-4E9B-B813-99F790CFD060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="175">
   <si>
     <t>Packet</t>
   </si>
@@ -516,6 +516,51 @@
   </si>
   <si>
     <t>Specific</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>insertion</t>
+  </si>
+  <si>
+    <t>clickEvent</t>
+  </si>
+  <si>
+    <t>hoverEvent</t>
+  </si>
+  <si>
+    <t>translate Component</t>
+  </si>
+  <si>
+    <t>keybind Component</t>
+  </si>
+  <si>
+    <t>score Component</t>
+  </si>
+  <si>
+    <t>convert to better names, Text.d.ts</t>
+  </si>
+  <si>
+    <t>convert to better names, implement item NBT, Tekst.d.ts</t>
+  </si>
+  <si>
+    <t>CustomError</t>
+  </si>
+  <si>
+    <t>expectationNotMet</t>
+  </si>
+  <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
+    <t>Action can't be performed right now</t>
+  </si>
+  <si>
+    <t>Can't set</t>
+  </si>
+  <si>
+    <t>chatToArray(</t>
   </si>
 </sst>
 </file>
@@ -755,13 +800,8 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="16">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -775,154 +815,14 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1029,83 +929,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3112,32 +2935,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D143">
-    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"Server"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"Client"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37 F34:F35 F20 F39 F41 F45 F5 F91 F112 F110 E5:E143 F123:F124 F9:F10 F47 F56">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Fully implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"Partly implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"Tried"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Not started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F110 E5:E143 F123:F124 F9:F10 F47 F56">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3151,16 +2974,16 @@
   <dimension ref="C2:F104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -3180,69 +3003,121 @@
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="F4" s="17"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
+      <c r="D6" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
+      <c r="C11" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.35">
@@ -3787,29 +3662,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E104">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Fully implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Partly implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Tried"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Not started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E104">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:F104">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="9">
       <formula>LEN(TRIM(C4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3853,7 +3728,7 @@
 +(COUNTIF(Miscellaneous!E4:E104,"not started")*Settings!D9)
 )/(ROWS(Packets!E5:E143+COUNTA(Miscellaneous!E4:E104))
 )*100)</f>
-        <v>26.258992805755394</v>
+        <v>28.201438848920869</v>
       </c>
     </row>
   </sheetData>
@@ -3870,7 +3745,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D34">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(C4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3884,7 +3759,7 @@
   <dimension ref="C4:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added <Entity>.remove to types
</commit_message>
<xml_diff>
--- a/progress/spreadsheet/spreadsheet.xlsx
+++ b/progress/spreadsheet/spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\progress\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ACF646-C629-4E9B-B813-99F790CFD060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE52F7C3-2E44-46AA-9EE8-EEB8599D3B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packets" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Stats" sheetId="2" r:id="rId3"/>
     <sheet name="Settings" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="174">
   <si>
     <t>Packet</t>
   </si>
@@ -504,9 +507,6 @@
   </si>
   <si>
     <t>translate, sender, position</t>
-  </si>
-  <si>
-    <t>q</t>
   </si>
   <si>
     <t>worlds, viewDistance, maxPlayers</t>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F143"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1447,9 +1447,7 @@
       <c r="E21" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>156</v>
-      </c>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C22" s="4" t="s">
@@ -1696,7 +1694,7 @@
         <v>140</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.35">
@@ -1903,7 +1901,7 @@
         <v>94</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F58" s="6"/>
     </row>
@@ -2973,7 +2971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEA0A1E-1012-46E5-BEEA-07D7C80FD93F}">
   <dimension ref="C2:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2990,10 +2988,10 @@
     <row r="2" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="3:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>158</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>2</v>
@@ -3004,10 +3002,10 @@
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C4" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>161</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>138</v>
@@ -3017,31 +3015,31 @@
     <row r="5" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C5" s="18"/>
       <c r="D5" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>140</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C6" s="18"/>
       <c r="D6" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>139</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C7" s="18"/>
       <c r="D7" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>139</v>
@@ -3051,7 +3049,7 @@
     <row r="8" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C8" s="18"/>
       <c r="D8" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>139</v>
@@ -3061,7 +3059,7 @@
     <row r="9" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C9" s="18"/>
       <c r="D9" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>139</v>
@@ -3071,7 +3069,7 @@
     <row r="10" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>139</v>
@@ -3080,10 +3078,10 @@
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C11" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>139</v>
@@ -3093,7 +3091,7 @@
     <row r="12" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>139</v>
@@ -3103,7 +3101,7 @@
     <row r="13" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C13" s="18"/>
       <c r="D13" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>139</v>
@@ -3113,7 +3111,7 @@
     <row r="14" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C14" s="18"/>
       <c r="D14" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>138</v>
@@ -3728,7 +3726,7 @@
 +(COUNTIF(Miscellaneous!E4:E104,"not started")*Settings!D9)
 )/(ROWS(Packets!E5:E143+COUNTA(Miscellaneous!E4:E104))
 )*100)</f>
-        <v>28.201438848920869</v>
+        <v>28.273381294964029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved and fixed bug in CustomError
</commit_message>
<xml_diff>
--- a/progress/spreadsheet/spreadsheet.xlsx
+++ b/progress/spreadsheet/spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\progress\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE52F7C3-2E44-46AA-9EE8-EEB8599D3B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5648E198-8743-4A1C-9A82-E3EDF5A14B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1481,7 +1481,7 @@
         <v>94</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="F24" s="6"/>
     </row>
@@ -1627,7 +1627,7 @@
         <v>94</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F36" s="6"/>
     </row>
@@ -3726,7 +3726,7 @@
 +(COUNTIF(Miscellaneous!E4:E104,"not started")*Settings!D9)
 )/(ROWS(Packets!E5:E143+COUNTA(Miscellaneous!E4:E104))
 )*100)</f>
-        <v>28.273381294964029</v>
+        <v>28.992805755395683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented loading bar in spreadsheet
</commit_message>
<xml_diff>
--- a/progress/spreadsheet/spreadsheet.xlsx
+++ b/progress/spreadsheet/spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\progress\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7AA7CD-897A-4A0D-B310-A39F8ABC0108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08771D00-9544-4D5F-BB99-0CD07032801C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Packets" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="173">
   <si>
     <t>Packet</t>
   </si>
@@ -545,9 +567,6 @@
     <t>expectationNotMet</t>
   </si>
   <si>
-    <t>Not implemented</t>
-  </si>
-  <si>
     <t>Action can't be performed right now</t>
   </si>
   <si>
@@ -558,12 +577,18 @@
   </si>
   <si>
     <t>see Text</t>
+  </si>
+  <si>
+    <t>length loading bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;;"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -736,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -793,11 +818,161 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1205,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129:E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1398,13 +1573,13 @@
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C18" s="4" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F18" s="6"/>
     </row>
@@ -1431,7 +1606,7 @@
         <v>138</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.35">
@@ -1952,13 +2127,13 @@
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C63" s="4" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F63" s="6"/>
     </row>
@@ -2942,32 +3117,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D144">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"Server"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"Client"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37 F34:F35 F20 F39 F41 F45 F5 F91 F113 F111 E5:E144 F124:F125 F9:F10 F47 F56">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"Fully implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"Partly implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>"Tried"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"Not started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F111 E5:E144 F124:F125 F9:F10 F47 F56">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2981,7 +3156,7 @@
   <dimension ref="C2:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3078,7 +3253,7 @@
     <row r="10" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>139</v>
@@ -3090,17 +3265,17 @@
         <v>166</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>139</v>
@@ -3110,7 +3285,7 @@
     <row r="13" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C13" s="18"/>
       <c r="D13" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>139</v>
@@ -3119,12 +3294,8 @@
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C14" s="18"/>
-      <c r="D14" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>138</v>
-      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.35">
@@ -3669,29 +3840,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:E104">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Fully implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Partly implemented"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"Tried"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Not started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E104">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"working"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:F104">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(C4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3702,10 +3873,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F031A1-1BAA-40E9-B49C-760E1954E8E5}">
-  <dimension ref="C4:D4"/>
+  <dimension ref="C4:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3716,12 +3887,12 @@
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="3">
-        <f>(
+      <c r="D4" s="3" cm="1">
+        <f t="array" ref="D4">(
 (
 (COUNTIF(Packets!E5:E144,"fully implemented")*Settings!D5)
 +(COUNTIF(Packets!E5:E144,"working implemented")*Settings!D6)
@@ -3738,9 +3909,142 @@
         <v>34.999999999999993</v>
       </c>
     </row>
+    <row r="6" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="D7" s="26">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0.59999999999999876</v>
+      </c>
+      <c r="J7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="27">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="28">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="29">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0.59999999999999876</v>
+      </c>
+      <c r="J8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="30">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="31">
+        <f>MAX(0, MIN(COLUMN()-3, D4/100*Settings!D12)-(COLUMN()-4))</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3751,22 +4055,34 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:D34">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="C4:D6 C9:D34 C7:C8">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(C4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D7:S8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="80"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA79DE60-9FBD-4AFE-B354-2911D8201B1C}">
-  <dimension ref="C4:D9"/>
+  <dimension ref="C4:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3792,7 +4108,7 @@
         <v>151</v>
       </c>
       <c r="D6">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.35">
@@ -3817,6 +4133,14 @@
       </c>
       <c r="D9">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled in spreadsheet with accurate values
</commit_message>
<xml_diff>
--- a/progress/spreadsheet/spreadsheet.xlsx
+++ b/progress/spreadsheet/spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\progress\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141FBC90-BB21-48A9-8695-8CAC81E7D6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E7A093-4FB2-4299-8231-CA2EAECC5DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="160">
   <si>
     <t>Packet</t>
   </si>
@@ -515,6 +515,9 @@
   </si>
   <si>
     <t>Tests</t>
+  </si>
+  <si>
+    <t>foodSaturation test</t>
   </si>
 </sst>
 </file>
@@ -1270,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1652,7 +1655,7 @@
         <v>138</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G27" s="12"/>
     </row>
@@ -1757,7 +1760,7 @@
         <v>138</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G34" s="12"/>
     </row>
@@ -2414,9 +2417,11 @@
         <v>138</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="G77" s="12"/>
+        <v>140</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="11" t="s">
@@ -2761,7 +2766,7 @@
         <v>136</v>
       </c>
       <c r="F100" s="24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G100" s="12"/>
     </row>
@@ -2971,7 +2976,7 @@
         <v>136</v>
       </c>
       <c r="F114" s="24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G114" s="12"/>
     </row>
@@ -3468,7 +3473,7 @@
   <dimension ref="C4:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3496,7 +3501,7 @@
     + (COUNTIF(Packets!F5:F143, "tried") * Settings!D8)
     + (COUNTIF(Packets!F5:F143, "not started") * Settings!D9)
   ) / (ROWS(Packets!E5:E143) * 2)</f>
-        <v>0.15683453237410069</v>
+        <v>0.16546762589928055</v>
       </c>
     </row>
     <row r="6" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3511,7 +3516,7 @@
       </c>
       <c r="F7" s="5">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
-        <v>0.5093525179856111</v>
+        <v>0.64748201438848874</v>
       </c>
       <c r="G7" s="5">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
@@ -3577,7 +3582,7 @@
       </c>
       <c r="F8" s="8">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
-        <v>0.5093525179856111</v>
+        <v>0.64748201438848874</v>
       </c>
       <c r="G8" s="8">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
@@ -3672,7 +3677,7 @@
   <dimension ref="C4:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated todo and spreadsheet
</commit_message>
<xml_diff>
--- a/progress/spreadsheet/spreadsheet.xlsx
+++ b/progress/spreadsheet/spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\Programmeren\minecraft-server\progress\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B2A315-A6B3-4FCC-B078-2238509BCE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE706B78-0410-4611-84E9-AFED143DA0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="161">
   <si>
     <t>Packet</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>foodSaturation test</t>
+  </si>
+  <si>
+    <t>update LoadedChunk based on what block is held</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1249,7 +1252,7 @@
     <col min="4" max="4" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -3377,12 +3380,14 @@
         <v>135</v>
       </c>
       <c r="E143" s="21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F143" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="G143" s="12"/>
+      <c r="G143" s="12" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="144" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C144" s="14" t="s">
@@ -3466,7 +3471,7 @@
     + (COUNTIF(Packets!F5:F143, "tried") * Settings!D8)
     + (COUNTIF(Packets!F5:F143, "not started") * Settings!D9)
   ) / (ROWS(Packets!E5:E143) * 2)</f>
-        <v>0.16546762589928055</v>
+        <v>0.16798561151079136</v>
       </c>
     </row>
     <row r="6" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3481,7 +3486,7 @@
       </c>
       <c r="F7" s="5">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
-        <v>0.64748201438848874</v>
+        <v>0.68776978417266177</v>
       </c>
       <c r="G7" s="5">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
@@ -3547,7 +3552,7 @@
       </c>
       <c r="F8" s="8">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>
-        <v>0.64748201438848874</v>
+        <v>0.68776978417266177</v>
       </c>
       <c r="G8" s="8">
         <f>MAX(0, MIN(COLUMN()-3, D4*Settings!D12)-(COLUMN()-4))</f>

</xml_diff>